<commit_message>
Edit template ubah nama kantor
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\KKPy\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\kkpy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44D546A9-FE64-4987-8C44-48597942531C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88CBFDB5-28A2-48F3-B7B2-56D46DBD7F48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19080" yWindow="2535" windowWidth="20730" windowHeight="11160" activeTab="7" xr2:uid="{37CF0A89-84A4-4790-A442-9A0C4627AC78}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" activeTab="5" xr2:uid="{37CF0A89-84A4-4790-A442-9A0C4627AC78}"/>
   </bookViews>
   <sheets>
     <sheet name="N" sheetId="3" r:id="rId1"/>
@@ -391,9 +391,6 @@
     <t>KERTAS KERJA PEMERIKSAAN</t>
   </si>
   <si>
-    <t>KANTOR PELAYANAN PAJAK PENANAMAN MODAL ASING EMPAT</t>
-  </si>
-  <si>
     <t>DIREKTORAT JENDERAL PAJAK</t>
   </si>
   <si>
@@ -470,6 +467,9 @@
   </si>
   <si>
     <t>Masa</t>
+  </si>
+  <si>
+    <t>NAMA KANTOR</t>
   </si>
 </sst>
 </file>
@@ -477,7 +477,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -697,11 +697,11 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -799,6 +799,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -808,16 +817,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1140,8 +1140,8 @@
   </sheetPr>
   <dimension ref="A1:R138"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A12" zoomScale="85" zoomScaleNormal="70" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView view="pageBreakPreview" zoomScale="85" zoomScaleNormal="70" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:R5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1157,17 +1157,17 @@
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="3" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>115</v>
+        <v>141</v>
       </c>
     </row>
     <row r="4" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1393,7 +1393,7 @@
         <v>105</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F15" s="5"/>
       <c r="G15" s="5"/>
@@ -1418,7 +1418,7 @@
         <v>95</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F16" s="5"/>
       <c r="G16" s="5"/>
@@ -1443,7 +1443,7 @@
         <v>94</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F17" s="5"/>
       <c r="G17" s="5"/>
@@ -1468,7 +1468,7 @@
         <v>93</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F18" s="5"/>
       <c r="G18" s="5"/>
@@ -1493,7 +1493,7 @@
         <v>92</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F19" s="5"/>
       <c r="G19" s="5"/>
@@ -1538,7 +1538,7 @@
         <v>103</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F21" s="5"/>
       <c r="G21" s="5"/>
@@ -1661,7 +1661,7 @@
       </c>
       <c r="D27" s="38"/>
       <c r="E27" s="13" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F27" s="13"/>
       <c r="G27" s="13"/>
@@ -1686,7 +1686,7 @@
         <v>82</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F28" s="5"/>
       <c r="G28" s="5"/>
@@ -1712,7 +1712,7 @@
       </c>
       <c r="D29" s="38"/>
       <c r="E29" s="13" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F29" s="13"/>
       <c r="G29" s="13"/>
@@ -1836,7 +1836,7 @@
         <v>95</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F35" s="5"/>
       <c r="G35" s="5"/>
@@ -1861,7 +1861,7 @@
         <v>94</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F36" s="5"/>
       <c r="G36" s="5"/>
@@ -1886,7 +1886,7 @@
         <v>93</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F37" s="5"/>
       <c r="G37" s="5"/>
@@ -1911,7 +1911,7 @@
         <v>92</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F38" s="5"/>
       <c r="G38" s="5"/>
@@ -2035,7 +2035,7 @@
         <v>88</v>
       </c>
       <c r="E44" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F44" s="5"/>
       <c r="G44" s="5"/>
@@ -2060,7 +2060,7 @@
         <v>87</v>
       </c>
       <c r="E45" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F45" s="5"/>
       <c r="G45" s="5"/>
@@ -2108,7 +2108,7 @@
         <v>84</v>
       </c>
       <c r="E47" s="13" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F47" s="13"/>
       <c r="G47" s="13"/>
@@ -2133,7 +2133,7 @@
         <v>82</v>
       </c>
       <c r="E48" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F48" s="5"/>
       <c r="G48" s="5"/>
@@ -2158,7 +2158,7 @@
         <v>80</v>
       </c>
       <c r="E49" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F49" s="5"/>
       <c r="G49" s="5"/>
@@ -2206,7 +2206,7 @@
         <v>76</v>
       </c>
       <c r="E51" s="5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F51" s="5"/>
       <c r="G51" s="5"/>
@@ -2231,7 +2231,7 @@
         <v>74</v>
       </c>
       <c r="E52" s="5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F52" s="5"/>
       <c r="G52" s="5"/>
@@ -3043,7 +3043,7 @@
     </row>
     <row r="94" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A94" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="95" spans="1:18" x14ac:dyDescent="0.2">
@@ -3152,7 +3152,7 @@
         <v>105</v>
       </c>
       <c r="E98" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F98" s="5"/>
       <c r="G98" s="5"/>
@@ -3177,7 +3177,7 @@
         <v>95</v>
       </c>
       <c r="E99" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F99" s="5"/>
       <c r="G99" s="5"/>
@@ -3202,7 +3202,7 @@
         <v>94</v>
       </c>
       <c r="E100" s="5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F100" s="5"/>
       <c r="G100" s="5"/>
@@ -3227,7 +3227,7 @@
         <v>93</v>
       </c>
       <c r="E101" s="5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F101" s="5"/>
       <c r="G101" s="5"/>
@@ -3252,7 +3252,7 @@
         <v>92</v>
       </c>
       <c r="E102" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F102" s="5"/>
       <c r="G102" s="5"/>
@@ -3297,7 +3297,7 @@
         <v>103</v>
       </c>
       <c r="E104" s="5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F104" s="5"/>
       <c r="G104" s="5"/>
@@ -3380,7 +3380,7 @@
       </c>
       <c r="D108" s="38"/>
       <c r="E108" s="13" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F108" s="13"/>
       <c r="G108" s="13"/>
@@ -3405,7 +3405,7 @@
         <v>82</v>
       </c>
       <c r="E109" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F109" s="5"/>
       <c r="G109" s="5"/>
@@ -3431,7 +3431,7 @@
       </c>
       <c r="D110" s="38"/>
       <c r="E110" s="13" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F110" s="13"/>
       <c r="G110" s="13"/>
@@ -3450,7 +3450,7 @@
     <row r="111" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A111" s="11"/>
       <c r="B111" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E111" s="5"/>
       <c r="F111" s="6"/>
@@ -3515,7 +3515,7 @@
         <v>95</v>
       </c>
       <c r="E114" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F114" s="5"/>
       <c r="G114" s="5"/>
@@ -3540,7 +3540,7 @@
         <v>94</v>
       </c>
       <c r="E115" s="5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F115" s="5"/>
       <c r="G115" s="5"/>
@@ -3565,7 +3565,7 @@
         <v>93</v>
       </c>
       <c r="E116" s="5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F116" s="5"/>
       <c r="G116" s="5"/>
@@ -3590,7 +3590,7 @@
         <v>92</v>
       </c>
       <c r="E117" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F117" s="5"/>
       <c r="G117" s="5"/>
@@ -3609,7 +3609,7 @@
     <row r="118" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A118" s="11"/>
       <c r="B118" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E118" s="5"/>
       <c r="F118" s="6"/>
@@ -3674,7 +3674,7 @@
         <v>88</v>
       </c>
       <c r="E121" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F121" s="5"/>
       <c r="G121" s="5"/>
@@ -3699,7 +3699,7 @@
         <v>87</v>
       </c>
       <c r="E122" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F122" s="5"/>
       <c r="G122" s="5"/>
@@ -3748,7 +3748,7 @@
         <v>84</v>
       </c>
       <c r="E124" s="13" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F124" s="13"/>
       <c r="G124" s="13"/>
@@ -3773,7 +3773,7 @@
         <v>82</v>
       </c>
       <c r="E125" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F125" s="5"/>
       <c r="G125" s="5"/>
@@ -3798,7 +3798,7 @@
         <v>80</v>
       </c>
       <c r="E126" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F126" s="5"/>
       <c r="G126" s="5"/>
@@ -3846,7 +3846,7 @@
         <v>76</v>
       </c>
       <c r="E128" s="5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F128" s="5"/>
       <c r="G128" s="5"/>
@@ -3871,7 +3871,7 @@
         <v>74</v>
       </c>
       <c r="E129" s="5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F129" s="5"/>
       <c r="G129" s="5"/>
@@ -3890,7 +3890,7 @@
     <row r="130" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A130" s="11"/>
       <c r="C130" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E130" s="5"/>
       <c r="F130" s="6"/>
@@ -3998,7 +3998,7 @@
         <v>24</v>
       </c>
       <c r="C135" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E135" s="5"/>
       <c r="F135" s="5"/>
@@ -4116,17 +4116,17 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>115</v>
+        <v>141</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
@@ -4192,37 +4192,37 @@
       <c r="A11" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="B11" s="50" t="s">
+      <c r="B11" s="47" t="s">
         <v>1</v>
       </c>
-      <c r="C11" s="47" t="s">
+      <c r="C11" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="D11" s="48"/>
+      <c r="D11" s="51"/>
       <c r="E11" s="46" t="s">
         <v>5</v>
       </c>
       <c r="F11" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="G11" s="51" t="s">
-        <v>141</v>
-      </c>
-      <c r="H11" s="47" t="s">
+      <c r="G11" s="48" t="s">
+        <v>140</v>
+      </c>
+      <c r="H11" s="50" t="s">
+        <v>134</v>
+      </c>
+      <c r="I11" s="51"/>
+      <c r="J11" s="50" t="s">
         <v>135</v>
       </c>
-      <c r="I11" s="48"/>
-      <c r="J11" s="47" t="s">
+      <c r="K11" s="51"/>
+      <c r="L11" s="50" t="s">
+        <v>137</v>
+      </c>
+      <c r="M11" s="52"/>
+      <c r="N11" s="51"/>
+      <c r="O11" s="46" t="s">
         <v>136</v>
-      </c>
-      <c r="K11" s="48"/>
-      <c r="L11" s="47" t="s">
-        <v>138</v>
-      </c>
-      <c r="M11" s="49"/>
-      <c r="N11" s="48"/>
-      <c r="O11" s="46" t="s">
-        <v>137</v>
       </c>
       <c r="P11" s="46" t="s">
         <v>71</v>
@@ -4230,7 +4230,7 @@
     </row>
     <row r="12" spans="1:16" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="46"/>
-      <c r="B12" s="50"/>
+      <c r="B12" s="47"/>
       <c r="C12" s="24" t="s">
         <v>4</v>
       </c>
@@ -4239,7 +4239,7 @@
       </c>
       <c r="E12" s="46"/>
       <c r="F12" s="46"/>
-      <c r="G12" s="52"/>
+      <c r="G12" s="49"/>
       <c r="H12" s="24" t="s">
         <v>4</v>
       </c>
@@ -4253,30 +4253,30 @@
         <v>14</v>
       </c>
       <c r="L12" s="24" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="M12" s="24" t="s">
         <v>3</v>
       </c>
       <c r="N12" s="24" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="O12" s="46"/>
       <c r="P12" s="46"/>
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="P11:P12"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="J11:K11"/>
+    <mergeCell ref="L11:N11"/>
     <mergeCell ref="A11:A12"/>
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="E11:E12"/>
     <mergeCell ref="F11:F12"/>
     <mergeCell ref="O11:O12"/>
     <mergeCell ref="G11:G12"/>
-    <mergeCell ref="P11:P12"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="J11:K11"/>
-    <mergeCell ref="L11:N11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="34" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
@@ -4306,7 +4306,7 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F1"/>
       <c r="G1"/>
@@ -4314,7 +4314,7 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F2"/>
       <c r="G2"/>
@@ -4322,7 +4322,7 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>115</v>
+        <v>141</v>
       </c>
       <c r="F3"/>
       <c r="G3"/>
@@ -4401,16 +4401,16 @@
       <c r="A11" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="50" t="s">
+      <c r="B11" s="47" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="50" t="s">
+      <c r="C11" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="D11" s="50" t="s">
+      <c r="D11" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="E11" s="50"/>
+      <c r="E11" s="47"/>
       <c r="F11" s="53" t="s">
         <v>5</v>
       </c>
@@ -4420,17 +4420,17 @@
       <c r="H11" s="53" t="s">
         <v>10</v>
       </c>
-      <c r="I11" s="50" t="s">
+      <c r="I11" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="J11" s="51" t="s">
-        <v>141</v>
+      <c r="J11" s="48" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="46"/>
-      <c r="B12" s="50"/>
-      <c r="C12" s="50"/>
+      <c r="B12" s="47"/>
+      <c r="C12" s="47"/>
       <c r="D12" s="35" t="s">
         <v>13</v>
       </c>
@@ -4440,8 +4440,8 @@
       <c r="F12" s="53"/>
       <c r="G12" s="53"/>
       <c r="H12" s="53"/>
-      <c r="I12" s="50"/>
-      <c r="J12" s="52"/>
+      <c r="I12" s="47"/>
+      <c r="J12" s="49"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -4471,17 +4471,17 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>115</v>
+        <v>141</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
@@ -4549,16 +4549,16 @@
       <c r="A11" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="50" t="s">
+      <c r="B11" s="47" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="50" t="s">
+      <c r="C11" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="D11" s="50" t="s">
+      <c r="D11" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="E11" s="50"/>
+      <c r="E11" s="47"/>
       <c r="F11" s="53" t="s">
         <v>5</v>
       </c>
@@ -4568,17 +4568,17 @@
       <c r="H11" s="53" t="s">
         <v>10</v>
       </c>
-      <c r="I11" s="50" t="s">
+      <c r="I11" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="J11" s="51" t="s">
-        <v>141</v>
+      <c r="J11" s="48" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="46"/>
-      <c r="B12" s="50"/>
-      <c r="C12" s="50"/>
+      <c r="B12" s="47"/>
+      <c r="C12" s="47"/>
       <c r="D12" s="35" t="s">
         <v>13</v>
       </c>
@@ -4588,8 +4588,8 @@
       <c r="F12" s="53"/>
       <c r="G12" s="53"/>
       <c r="H12" s="53"/>
-      <c r="I12" s="50"/>
-      <c r="J12" s="52"/>
+      <c r="I12" s="47"/>
+      <c r="J12" s="49"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -4626,17 +4626,17 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>115</v>
+        <v>141</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
@@ -4704,16 +4704,16 @@
       <c r="A11" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="50" t="s">
+      <c r="B11" s="47" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="50" t="s">
+      <c r="C11" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="D11" s="50" t="s">
+      <c r="D11" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="E11" s="50"/>
+      <c r="E11" s="47"/>
       <c r="F11" s="53" t="s">
         <v>5</v>
       </c>
@@ -4723,17 +4723,17 @@
       <c r="H11" s="53" t="s">
         <v>10</v>
       </c>
-      <c r="I11" s="50" t="s">
+      <c r="I11" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="J11" s="51" t="s">
-        <v>141</v>
+      <c r="J11" s="48" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="46"/>
-      <c r="B12" s="50"/>
-      <c r="C12" s="50"/>
+      <c r="B12" s="47"/>
+      <c r="C12" s="47"/>
       <c r="D12" s="35" t="s">
         <v>13</v>
       </c>
@@ -4743,8 +4743,8 @@
       <c r="F12" s="53"/>
       <c r="G12" s="53"/>
       <c r="H12" s="53"/>
-      <c r="I12" s="50"/>
-      <c r="J12" s="52"/>
+      <c r="I12" s="47"/>
+      <c r="J12" s="49"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -4766,7 +4766,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D80082AC-6168-4EC5-B599-1197EDE6463A}">
   <dimension ref="A1:O12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:XFD12"/>
     </sheetView>
   </sheetViews>
@@ -4774,17 +4774,17 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>115</v>
+        <v>141</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
@@ -4852,16 +4852,16 @@
       <c r="A11" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="50" t="s">
+      <c r="B11" s="47" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="50" t="s">
+      <c r="C11" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="D11" s="50" t="s">
+      <c r="D11" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="E11" s="50"/>
+      <c r="E11" s="47"/>
       <c r="F11" s="53" t="s">
         <v>5</v>
       </c>
@@ -4871,17 +4871,17 @@
       <c r="H11" s="53" t="s">
         <v>10</v>
       </c>
-      <c r="I11" s="50" t="s">
+      <c r="I11" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="J11" s="51" t="s">
-        <v>141</v>
+      <c r="J11" s="48" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="46"/>
-      <c r="B12" s="50"/>
-      <c r="C12" s="50"/>
+      <c r="B12" s="47"/>
+      <c r="C12" s="47"/>
       <c r="D12" s="35" t="s">
         <v>13</v>
       </c>
@@ -4891,8 +4891,8 @@
       <c r="F12" s="53"/>
       <c r="G12" s="53"/>
       <c r="H12" s="53"/>
-      <c r="I12" s="50"/>
-      <c r="J12" s="52"/>
+      <c r="I12" s="47"/>
+      <c r="J12" s="49"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -4922,17 +4922,17 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>115</v>
+        <v>141</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
@@ -5000,16 +5000,16 @@
       <c r="A11" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="50" t="s">
+      <c r="B11" s="47" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="50" t="s">
+      <c r="C11" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="D11" s="50" t="s">
+      <c r="D11" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="E11" s="50"/>
+      <c r="E11" s="47"/>
       <c r="F11" s="53" t="s">
         <v>5</v>
       </c>
@@ -5019,17 +5019,17 @@
       <c r="H11" s="53" t="s">
         <v>10</v>
       </c>
-      <c r="I11" s="50" t="s">
+      <c r="I11" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="J11" s="51" t="s">
-        <v>141</v>
+      <c r="J11" s="48" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="46"/>
-      <c r="B12" s="50"/>
-      <c r="C12" s="50"/>
+      <c r="B12" s="47"/>
+      <c r="C12" s="47"/>
       <c r="D12" s="35" t="s">
         <v>13</v>
       </c>
@@ -5039,8 +5039,8 @@
       <c r="F12" s="53"/>
       <c r="G12" s="53"/>
       <c r="H12" s="53"/>
-      <c r="I12" s="50"/>
-      <c r="J12" s="52"/>
+      <c r="I12" s="47"/>
+      <c r="J12" s="49"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -5062,7 +5062,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C9BEC2F-90B0-4B37-8774-E50C26A13D48}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>

</xml_diff>